<commit_message>
files and logs used to produce CR_itemshape_2_20170124.zip
</commit_message>
<xml_diff>
--- a/publication/part1000/CR_itemshape_2/Bugzilla_list.xlsx
+++ b/publication/part1000/CR_itemshape_2/Bugzilla_list.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27815"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460"/>
+    <workbookView xWindow="700" yWindow="-24000" windowWidth="28800" windowHeight="17460"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="1" r:id="rId1"/>
@@ -1826,7 +1826,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K94" sqref="K94"/>
+      <selection pane="bottomLeft" activeCell="G53" sqref="G53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1836,11 +1836,11 @@
     <col min="3" max="3" width="17.5" style="4" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="29.6640625" style="19" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="52" style="19" customWidth="1"/>
-    <col min="6" max="6" width="18.33203125" style="7" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="21.1640625" style="4" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="19.1640625" style="4" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="45.5" style="4" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="7.6640625" style="4" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" style="7" customWidth="1"/>
+    <col min="7" max="7" width="21.1640625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="19.1640625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="45.5" style="4" customWidth="1"/>
+    <col min="10" max="10" width="7.6640625" style="4" customWidth="1"/>
     <col min="11" max="11" width="14.5" style="4" customWidth="1"/>
     <col min="12" max="12" width="100.33203125" style="2" customWidth="1"/>
     <col min="13" max="13" width="10.1640625" style="2" customWidth="1"/>

</xml_diff>